<commit_message>
add gpt 4o and latency/token plots
</commit_message>
<xml_diff>
--- a/llmcompanion/all_latency_05.01.xlsx
+++ b/llmcompanion/all_latency_05.01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onurd\Desktop\CMPE491\llmcompanion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34976FF0-80B5-494F-B800-DDCC156463D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3CF184-C36C-4A68-8CAA-9B5E93AEB50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>Success</t>
   </si>
   <si>
-    <t>publishers/meta/models/llama-3.1-8b-instruct-maas</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -462,6 +459,9 @@
   </si>
   <si>
     <t>4.379347085952759</t>
+  </si>
+  <si>
+    <t>llama-3.1-8b-instruct-maas</t>
   </si>
 </sst>
 </file>
@@ -782,11 +782,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -819,16 +822,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -843,22 +846,22 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
@@ -872,21 +875,21 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -901,22 +904,22 @@
         <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
@@ -930,22 +933,22 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
@@ -959,21 +962,21 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -988,22 +991,22 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
@@ -1017,22 +1020,22 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
@@ -1046,22 +1049,22 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
@@ -1075,22 +1078,22 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
@@ -1104,18 +1107,18 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>7.4307358264923096</v>
@@ -1130,25 +1133,25 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
@@ -1162,22 +1165,22 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
@@ -1191,22 +1194,22 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
@@ -1220,22 +1223,22 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
@@ -1249,22 +1252,22 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
@@ -1278,18 +1281,18 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>8.4562323093414307</v>
@@ -1307,22 +1310,22 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
@@ -1336,22 +1339,22 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
@@ -1365,22 +1368,22 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E21" t="b">
         <v>0</v>
       </c>
@@ -1391,22 +1394,22 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="E22" t="b">
         <v>0</v>
       </c>
@@ -1417,22 +1420,22 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
@@ -1446,22 +1449,22 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
@@ -1472,22 +1475,22 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E25" t="b">
         <v>0</v>
       </c>
@@ -1501,22 +1504,22 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E26" t="b">
         <v>0</v>
       </c>
@@ -1530,22 +1533,22 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
@@ -1556,18 +1559,18 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28">
         <v>6.033935546875</v>
@@ -1585,22 +1588,22 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="E29" t="b">
         <v>0</v>
       </c>
@@ -1611,22 +1614,22 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="E30" t="b">
         <v>0</v>
       </c>
@@ -1640,21 +1643,21 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1669,21 +1672,21 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1698,22 +1701,22 @@
         <v>6</v>
       </c>
       <c r="I32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E33" t="b">
         <v>0</v>
       </c>
@@ -1724,21 +1727,21 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1753,22 +1756,22 @@
         <v>22</v>
       </c>
       <c r="I34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E35" t="b">
         <v>0</v>
       </c>
@@ -1782,21 +1785,21 @@
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1811,22 +1814,22 @@
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E37" t="b">
         <v>0</v>
       </c>
@@ -1840,21 +1843,21 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1869,21 +1872,21 @@
         <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1898,22 +1901,22 @@
         <v>5</v>
       </c>
       <c r="I39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="E40" t="b">
         <v>0</v>
       </c>
@@ -1927,22 +1930,22 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E41" t="b">
         <v>0</v>
       </c>
@@ -1953,22 +1956,22 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="E42" t="b">
         <v>0</v>
       </c>
@@ -1979,22 +1982,22 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="E43" t="b">
         <v>0</v>
       </c>
@@ -2005,18 +2008,18 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44">
         <v>9.9857416152954102</v>
@@ -2034,22 +2037,22 @@
         <v>13</v>
       </c>
       <c r="I44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="E45" t="b">
         <v>0</v>
       </c>
@@ -2063,22 +2066,22 @@
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E46" t="b">
         <v>0</v>
       </c>
@@ -2089,22 +2092,22 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
@@ -2115,22 +2118,22 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E48" t="b">
         <v>0</v>
       </c>
@@ -2141,22 +2144,22 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="E49" t="b">
         <v>0</v>
       </c>
@@ -2167,22 +2170,22 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="E50" t="b">
         <v>0</v>
       </c>
@@ -2193,21 +2196,21 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2222,22 +2225,22 @@
         <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="E52" t="b">
         <v>0</v>
       </c>
@@ -2251,22 +2254,22 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="E53" t="b">
         <v>0</v>
       </c>
@@ -2277,22 +2280,22 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="E54" t="b">
         <v>0</v>
       </c>
@@ -2303,22 +2306,22 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C55" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="E55" t="b">
         <v>0</v>
       </c>
@@ -2329,22 +2332,22 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="E56" t="b">
         <v>0</v>
       </c>
@@ -2358,22 +2361,22 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="E57" t="b">
         <v>0</v>
       </c>
@@ -2381,22 +2384,22 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="E58" t="b">
         <v>0</v>
       </c>
@@ -2404,22 +2407,22 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="E59" t="b">
         <v>0</v>
       </c>
@@ -2427,22 +2430,22 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="E60" t="b">
         <v>0</v>
       </c>
@@ -2450,22 +2453,22 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="E61" t="b">
         <v>0</v>
       </c>
@@ -2473,22 +2476,22 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="E62" t="b">
         <v>0</v>
       </c>
@@ -2496,22 +2499,22 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E63" t="b">
         <v>0</v>
       </c>
@@ -2519,22 +2522,22 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="E64" t="b">
         <v>0</v>
       </c>
@@ -2542,22 +2545,22 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s">
+        <v>135</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="E65" t="b">
         <v>0</v>
       </c>
@@ -2565,22 +2568,22 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="E66" t="b">
         <v>0</v>
       </c>
@@ -2588,22 +2591,22 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="E67" t="b">
         <v>0</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>